<commit_message>
fixing the names for TOR450
</commit_message>
<xml_diff>
--- a/TOR450 Data/5. Clean Data for Data Visualisation/TOR450_dem.xlsx
+++ b/TOR450 Data/5. Clean Data for Data Visualisation/TOR450_dem.xlsx
@@ -76,9 +76,9 @@
 3      4072
 4      4137
        ... 
-552    4034
-553    4039
-554    4051
+552    4014
+553    4034
+554    4039
 555    4016
 556    4047
 Name: Bib, Length: 557, dtype: object</t>
@@ -90,9 +90,9 @@
 3      4072
 4      4137
        ... 
-552    4034
-553    4039
-554    4051
+552    4014
+553    4034
+554    4039
 555    4016
 556    4047
 Name: Bib, Length: 557, dtype: object</t>
@@ -104,9 +104,9 @@
 3      4072
 4      4137
        ... 
-552    4034
-553    4039
-554    4051
+552    4014
+553    4034
+554    4039
 555    4016
 556    4047
 Name: Bib, Length: 557, dtype: object</t>
@@ -118,9 +118,9 @@
 3      4072
 4      4137
        ... 
-552    4034
-553    4039
-554    4051
+552    4014
+553    4034
+554    4039
 555    4016
 556    4047
 Name: Bib, Length: 557, dtype: object</t>
@@ -249,15 +249,15 @@
     <t>4143</t>
   </si>
   <si>
+    <t>4011</t>
+  </si>
+  <si>
     <t>4141</t>
   </si>
   <si>
     <t>4022</t>
   </si>
   <si>
-    <t>4011</t>
-  </si>
-  <si>
     <t>4130</t>
   </si>
   <si>
@@ -384,6 +384,9 @@
     <t>4076</t>
   </si>
   <si>
+    <t>4068</t>
+  </si>
+  <si>
     <t>4098</t>
   </si>
   <si>
@@ -399,21 +402,21 @@
     <t>4119</t>
   </si>
   <si>
+    <t>4111</t>
+  </si>
+  <si>
+    <t>4093</t>
+  </si>
+  <si>
+    <t>4003</t>
+  </si>
+  <si>
+    <t>4099</t>
+  </si>
+  <si>
     <t>4069</t>
   </si>
   <si>
-    <t>4111</t>
-  </si>
-  <si>
-    <t>4093</t>
-  </si>
-  <si>
-    <t>4003</t>
-  </si>
-  <si>
-    <t>4099</t>
-  </si>
-  <si>
     <t>4065</t>
   </si>
   <si>
@@ -447,9 +450,6 @@
     <t>4028</t>
   </si>
   <si>
-    <t>4068</t>
-  </si>
-  <si>
     <t>4083</t>
   </si>
   <si>
@@ -765,7 +765,7 @@
     <t>Brussolo Simone</t>
   </si>
   <si>
-    <t>Buitrago Rodriguez Oscar Javier</t>
+    <t>Buitrago Javier</t>
   </si>
   <si>
     <t>Callisardi Giancarlo</t>
@@ -810,7 +810,10 @@
     <t>Defecinski Radoslaw</t>
   </si>
   <si>
-    <t>Devine Keri Ann</t>
+    <t>Devine Keri</t>
+  </si>
+  <si>
+    <t>Domnin Erard</t>
   </si>
   <si>
     <t>Dorne Franck</t>
@@ -819,9 +822,6 @@
     <t>Ekse Kaisa</t>
   </si>
   <si>
-    <t>Erard Domnin</t>
-  </si>
-  <si>
     <t>Erwee Tiaan</t>
   </si>
   <si>
@@ -843,7 +843,7 @@
     <t>Gasparini Thierry</t>
   </si>
   <si>
-    <t>Geist William</t>
+    <t>Geist Bill</t>
   </si>
   <si>
     <t>Gentilini Iader</t>
@@ -858,13 +858,13 @@
     <t>Goeringer Patrick</t>
   </si>
   <si>
-    <t>Gong Ming Cheng (Tom)</t>
+    <t>Gong Mingcheng</t>
   </si>
   <si>
     <t>Gosney Brett</t>
   </si>
   <si>
-    <t>Gosney Missy</t>
+    <t>Gosney Melissa</t>
   </si>
   <si>
     <t>Guasina Giorgio</t>
@@ -909,7 +909,7 @@
     <t>Humphrey Andy</t>
   </si>
   <si>
-    <t>Iancu David Traian</t>
+    <t>Iancu David</t>
   </si>
   <si>
     <t>Iotti Sebastien</t>
@@ -948,6 +948,9 @@
     <t>Locatelli Michele Oriele</t>
   </si>
   <si>
+    <t>Madeira Luis</t>
+  </si>
+  <si>
     <t>Mallol Luc</t>
   </si>
   <si>
@@ -963,9 +966,6 @@
     <t>Marquis Micha</t>
   </si>
   <si>
-    <t>Martinez Rodriguez Jose</t>
-  </si>
-  <si>
     <t>Michaud Andre Paul</t>
   </si>
   <si>
@@ -978,6 +978,9 @@
     <t>Mousseaux David</t>
   </si>
   <si>
+    <t>Mrtinez Jose</t>
+  </si>
+  <si>
     <t>Negri Mattia</t>
   </si>
   <si>
@@ -1011,9 +1014,6 @@
     <t>Piazzo Mario</t>
   </si>
   <si>
-    <t>Picanco Madeira Luis Manuel</t>
-  </si>
-  <si>
     <t>Pivert Jean Baptiste</t>
   </si>
   <si>
@@ -1041,7 +1041,7 @@
     <t>Raichon Sebastien</t>
   </si>
   <si>
-    <t>Ramos Quispe Mario Wilbert</t>
+    <t>Ramos Mario</t>
   </si>
   <si>
     <t>Rao Shashwat</t>
@@ -1053,7 +1053,7 @@
     <t>Rizzo Diego</t>
   </si>
   <si>
-    <t>Roig Carcel Josep</t>
+    <t>Roig Josep</t>
   </si>
   <si>
     <t>Rosati Luciano</t>
@@ -1146,7 +1146,7 @@
     <t>Annovazzi Giancarlo</t>
   </si>
   <si>
-    <t>Antonin Claudio Roger</t>
+    <t>Antonin Claudio</t>
   </si>
   <si>
     <t>Argelich Torra Enrique</t>
@@ -1227,7 +1227,7 @@
     <t>Comero Roberto</t>
   </si>
   <si>
-    <t>Compagnoni Gustavo Fernando</t>
+    <t>Compagnoni Gustavo</t>
   </si>
   <si>
     <t>Crussy Thierry</t>
@@ -1242,7 +1242,7 @@
     <t>Danet Fabien</t>
   </si>
   <si>
-    <t>De Santiago Iglesias Luis Angel</t>
+    <t>De Santiago Luis</t>
   </si>
   <si>
     <t>Demeter Michal</t>
@@ -1305,6 +1305,9 @@
     <t>Forzani Adriano</t>
   </si>
   <si>
+    <t>Frederic Gil</t>
+  </si>
+  <si>
     <t>Gaffuri Paolo</t>
   </si>
   <si>
@@ -1314,9 +1317,6 @@
     <t>Giacchetta Stephane</t>
   </si>
   <si>
-    <t>Gil Frederic</t>
-  </si>
-  <si>
     <t>Giovannini Giacomo</t>
   </si>
   <si>
@@ -1335,7 +1335,7 @@
     <t>Gueraud Laurent</t>
   </si>
   <si>
-    <t>Hayes Steven</t>
+    <t>Hayes Steve</t>
   </si>
   <si>
     <t>Haylett Philip</t>
@@ -1344,7 +1344,7 @@
     <t>Hernandez Ruiz Javier</t>
   </si>
   <si>
-    <t>Herrero Casas Albert</t>
+    <t>Herrero Albert</t>
   </si>
   <si>
     <t>Herrmann Sebastien</t>
@@ -1449,6 +1449,9 @@
     <t>Pettinato Filippo</t>
   </si>
   <si>
+    <t>Pierre Selva</t>
+  </si>
+  <si>
     <t>Podraza Tadeusz</t>
   </si>
   <si>
@@ -1497,9 +1500,6 @@
     <t>Santos Nuno</t>
   </si>
   <si>
-    <t>Selva Pierre</t>
-  </si>
-  <si>
     <t>Shao Sebastien</t>
   </si>
   <si>
@@ -1605,7 +1605,7 @@
     <t>De Biase Anna</t>
   </si>
   <si>
-    <t>De Lahitte Hernan Roberto</t>
+    <t>De Lahitte Hernan</t>
   </si>
   <si>
     <t>De Marco Enrico</t>
@@ -1713,7 +1713,7 @@
     <t>Luboz Dante</t>
   </si>
   <si>
-    <t>Madrigal Moya Ligia</t>
+    <t>Madrigal Ligia</t>
   </si>
   <si>
     <t>Maistri Francesco</t>
@@ -1734,7 +1734,7 @@
     <t>Olivson Oleksandr</t>
   </si>
   <si>
-    <t>Ong Soon Seng (Steven)</t>
+    <t>Ong Soonseng</t>
   </si>
   <si>
     <t>Ost Vincent</t>
@@ -1743,7 +1743,7 @@
     <t>Paschetto Renzo</t>
   </si>
   <si>
-    <t>Perrone Fodaro Carmelo</t>
+    <t>Perrone Carmelo</t>
   </si>
   <si>
     <t>Pirovano Andrea</t>
@@ -1764,7 +1764,7 @@
     <t>Ralcheva Aneta</t>
   </si>
   <si>
-    <t>Rastelli Daniel Fernando</t>
+    <t>Rastelli Daniel</t>
   </si>
   <si>
     <t>Richard Yann</t>
@@ -1791,6 +1791,9 @@
     <t>Teuscher Christof</t>
   </si>
   <si>
+    <t>Timo Vogel</t>
+  </si>
+  <si>
     <t>Turin Nicholas</t>
   </si>
   <si>
@@ -1803,9 +1806,6 @@
     <t>Villa Simone</t>
   </si>
   <si>
-    <t>Vogel Timo</t>
-  </si>
-  <si>
     <t>Wijaya Hendra</t>
   </si>
   <si>
@@ -1833,6 +1833,9 @@
     <t>Dufour Olivier</t>
   </si>
   <si>
+    <t>Eric Jeanclaude</t>
+  </si>
+  <si>
     <t>Ferrari Fabio</t>
   </si>
   <si>
@@ -1848,13 +1851,13 @@
     <t>Holst Benjamin</t>
   </si>
   <si>
+    <t>Jan Kriska</t>
+  </si>
+  <si>
     <t>Javega David</t>
   </si>
   <si>
-    <t>Jeanclaude Eric</t>
-  </si>
-  <si>
-    <t>Kriska Jan</t>
+    <t>Jose Urizar</t>
   </si>
   <si>
     <t>L Heureux Yvan</t>
@@ -1863,7 +1866,7 @@
     <t>Macchiavello Giorgio</t>
   </si>
   <si>
-    <t>Marzotto Ita Emanuela Anna</t>
+    <t>Marzotto Ita Emanuela</t>
   </si>
   <si>
     <t>Matthieu Moreau</t>
@@ -1872,7 +1875,7 @@
     <t>Neale Matt</t>
   </si>
   <si>
-    <t>Petersen Heine Hove</t>
+    <t>Petersen Heine</t>
   </si>
   <si>
     <t>Philippe Perez</t>
@@ -1894,9 +1897,6 @@
   </si>
   <si>
     <t>Szymik Marcin</t>
-  </si>
-  <si>
-    <t>Urizar Jose Lorenzo</t>
   </si>
   <si>
     <t>Vincent Wendling</t>
@@ -3908,7 +3908,7 @@
         <v>617</v>
       </c>
       <c r="H38" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="I38" t="s">
         <v>675</v>
@@ -3937,13 +3937,13 @@
         <v>252</v>
       </c>
       <c r="F39" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="G39" t="s">
-        <v>634</v>
+        <v>617</v>
       </c>
       <c r="H39" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="I39" t="s">
         <v>675</v>
@@ -3972,13 +3972,13 @@
         <v>253</v>
       </c>
       <c r="F40" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="G40" t="s">
-        <v>617</v>
+        <v>634</v>
       </c>
       <c r="H40" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="I40" t="s">
         <v>675</v>
@@ -4019,10 +4019,10 @@
         <v>674</v>
       </c>
       <c r="K41">
-        <v>134.3930555555556</v>
+        <v>134.3930555555555</v>
       </c>
       <c r="L41">
-        <v>483815.0000000001</v>
+        <v>483815</v>
       </c>
       <c r="M41" t="s">
         <v>682</v>
@@ -5570,10 +5570,10 @@
         <v>614</v>
       </c>
       <c r="G83" t="s">
-        <v>617</v>
+        <v>636</v>
       </c>
       <c r="H83" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="I83" t="s">
         <v>675</v>
@@ -5605,10 +5605,10 @@
         <v>614</v>
       </c>
       <c r="G84" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="H84" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="I84" t="s">
         <v>675</v>
@@ -5640,22 +5640,16 @@
         <v>614</v>
       </c>
       <c r="G85" t="s">
-        <v>617</v>
+        <v>621</v>
       </c>
       <c r="H85" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="I85" t="s">
-        <v>674</v>
-      </c>
-      <c r="K85">
-        <v>162.8666666666667</v>
-      </c>
-      <c r="L85">
-        <v>586320</v>
+        <v>675</v>
       </c>
       <c r="M85" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="Q85" t="s">
         <v>675</v>
@@ -5678,19 +5672,25 @@
         <v>299</v>
       </c>
       <c r="F86" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="G86" t="s">
-        <v>641</v>
+        <v>617</v>
       </c>
       <c r="H86" t="s">
-        <v>669</v>
+        <v>672</v>
       </c>
       <c r="I86" t="s">
-        <v>675</v>
+        <v>674</v>
+      </c>
+      <c r="K86">
+        <v>162.8666666666667</v>
+      </c>
+      <c r="L86">
+        <v>586320</v>
       </c>
       <c r="M86" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="Q86" t="s">
         <v>675</v>
@@ -5713,13 +5713,13 @@
         <v>300</v>
       </c>
       <c r="F87" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="G87" t="s">
-        <v>617</v>
+        <v>641</v>
       </c>
       <c r="H87" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="I87" t="s">
         <v>675</v>
@@ -5751,10 +5751,10 @@
         <v>614</v>
       </c>
       <c r="G88" t="s">
-        <v>630</v>
+        <v>617</v>
       </c>
       <c r="H88" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="I88" t="s">
         <v>675</v>
@@ -5932,10 +5932,10 @@
         <v>614</v>
       </c>
       <c r="G93" t="s">
-        <v>621</v>
+        <v>630</v>
       </c>
       <c r="H93" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="I93" t="s">
         <v>675</v>
@@ -5964,13 +5964,13 @@
         <v>307</v>
       </c>
       <c r="F94" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="G94" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="H94" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="I94" t="s">
         <v>675</v>
@@ -5999,10 +5999,10 @@
         <v>308</v>
       </c>
       <c r="F95" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="G95" t="s">
-        <v>621</v>
+        <v>634</v>
       </c>
       <c r="H95" t="s">
         <v>670</v>
@@ -6037,10 +6037,10 @@
         <v>614</v>
       </c>
       <c r="G96" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="H96" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="I96" t="s">
         <v>675</v>
@@ -6072,7 +6072,7 @@
         <v>614</v>
       </c>
       <c r="G97" t="s">
-        <v>617</v>
+        <v>625</v>
       </c>
       <c r="H97" t="s">
         <v>669</v>
@@ -6104,25 +6104,19 @@
         <v>311</v>
       </c>
       <c r="F98" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="G98" t="s">
-        <v>625</v>
+        <v>617</v>
       </c>
       <c r="H98" t="s">
         <v>669</v>
       </c>
       <c r="I98" t="s">
-        <v>674</v>
-      </c>
-      <c r="K98">
-        <v>168.0755555555556</v>
-      </c>
-      <c r="L98">
-        <v>605072</v>
+        <v>675</v>
       </c>
       <c r="M98" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="Q98" t="s">
         <v>675</v>
@@ -6145,19 +6139,25 @@
         <v>312</v>
       </c>
       <c r="F99" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="G99" t="s">
-        <v>621</v>
+        <v>625</v>
       </c>
       <c r="H99" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="I99" t="s">
-        <v>675</v>
+        <v>674</v>
+      </c>
+      <c r="K99">
+        <v>168.0755555555556</v>
+      </c>
+      <c r="L99">
+        <v>605072</v>
       </c>
       <c r="M99" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="Q99" t="s">
         <v>675</v>
@@ -6183,22 +6183,16 @@
         <v>614</v>
       </c>
       <c r="G100" t="s">
-        <v>617</v>
+        <v>621</v>
       </c>
       <c r="H100" t="s">
         <v>670</v>
       </c>
       <c r="I100" t="s">
-        <v>674</v>
-      </c>
-      <c r="K100">
-        <v>183.2702777777778</v>
-      </c>
-      <c r="L100">
-        <v>659773</v>
+        <v>675</v>
       </c>
       <c r="M100" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="Q100" t="s">
         <v>675</v>
@@ -6227,19 +6221,19 @@
         <v>617</v>
       </c>
       <c r="H101" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="I101" t="s">
         <v>674</v>
       </c>
       <c r="K101">
-        <v>134.3933333333333</v>
+        <v>183.2702777777778</v>
       </c>
       <c r="L101">
-        <v>483816.0000000001</v>
+        <v>659773</v>
       </c>
       <c r="M101" t="s">
-        <v>682</v>
+        <v>677</v>
       </c>
       <c r="Q101" t="s">
         <v>675</v>
@@ -6265,16 +6259,22 @@
         <v>614</v>
       </c>
       <c r="G102" t="s">
-        <v>642</v>
+        <v>617</v>
       </c>
       <c r="H102" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="I102" t="s">
-        <v>675</v>
+        <v>674</v>
+      </c>
+      <c r="K102">
+        <v>134.3933333333333</v>
+      </c>
+      <c r="L102">
+        <v>483816</v>
       </c>
       <c r="M102" t="s">
-        <v>678</v>
+        <v>682</v>
       </c>
       <c r="Q102" t="s">
         <v>675</v>
@@ -6300,10 +6300,10 @@
         <v>614</v>
       </c>
       <c r="G103" t="s">
-        <v>621</v>
+        <v>642</v>
       </c>
       <c r="H103" t="s">
-        <v>669</v>
+        <v>672</v>
       </c>
       <c r="I103" t="s">
         <v>675</v>
@@ -6335,10 +6335,10 @@
         <v>614</v>
       </c>
       <c r="G104" t="s">
-        <v>636</v>
+        <v>621</v>
       </c>
       <c r="H104" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="I104" t="s">
         <v>675</v>
@@ -7518,7 +7518,7 @@
         <v>136.3888888888889</v>
       </c>
       <c r="L136">
-        <v>491000.0000000001</v>
+        <v>491000</v>
       </c>
       <c r="M136" t="s">
         <v>682</v>
@@ -7836,7 +7836,7 @@
         <v>24</v>
       </c>
       <c r="D145" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E145" t="s">
         <v>358</v>
@@ -8169,7 +8169,7 @@
         <v>24</v>
       </c>
       <c r="D154" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E154" t="s">
         <v>364</v>
@@ -8444,7 +8444,7 @@
         <v>24</v>
       </c>
       <c r="D161" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E161" t="s">
         <v>370</v>
@@ -8590,7 +8590,7 @@
         <v>24</v>
       </c>
       <c r="D165" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E165" t="s">
         <v>374</v>
@@ -8888,7 +8888,7 @@
         <v>24</v>
       </c>
       <c r="D173" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E173" t="s">
         <v>236</v>
@@ -9332,7 +9332,7 @@
         <v>24</v>
       </c>
       <c r="D185" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="E185" t="s">
         <v>387</v>
@@ -9729,7 +9729,7 @@
         <v>24</v>
       </c>
       <c r="D196" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E196" t="s">
         <v>398</v>
@@ -9770,7 +9770,7 @@
         <v>24</v>
       </c>
       <c r="D197" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E197" t="s">
         <v>399</v>
@@ -9890,19 +9890,19 @@
         <v>24</v>
       </c>
       <c r="D200" t="s">
-        <v>156</v>
+        <v>68</v>
       </c>
       <c r="E200" t="s">
-        <v>402</v>
+        <v>251</v>
       </c>
       <c r="F200" t="s">
         <v>614</v>
       </c>
       <c r="G200" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="H200" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="I200" t="s">
         <v>675</v>
@@ -9925,19 +9925,19 @@
         <v>24</v>
       </c>
       <c r="D201" t="s">
-        <v>183</v>
+        <v>156</v>
       </c>
       <c r="E201" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F201" t="s">
         <v>614</v>
       </c>
       <c r="G201" t="s">
-        <v>617</v>
+        <v>621</v>
       </c>
       <c r="H201" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="I201" t="s">
         <v>675</v>
@@ -9960,31 +9960,25 @@
         <v>24</v>
       </c>
       <c r="D202" t="s">
-        <v>149</v>
+        <v>183</v>
       </c>
       <c r="E202" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F202" t="s">
         <v>614</v>
       </c>
       <c r="G202" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="H202" t="s">
         <v>669</v>
       </c>
       <c r="I202" t="s">
-        <v>674</v>
-      </c>
-      <c r="K202">
-        <v>188.4816666666667</v>
-      </c>
-      <c r="L202">
-        <v>678534</v>
+        <v>675</v>
       </c>
       <c r="M202" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="Q202" t="s">
         <v>675</v>
@@ -10001,25 +9995,31 @@
         <v>24</v>
       </c>
       <c r="D203" t="s">
-        <v>52</v>
+        <v>149</v>
       </c>
       <c r="E203" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F203" t="s">
         <v>614</v>
       </c>
       <c r="G203" t="s">
-        <v>636</v>
+        <v>621</v>
       </c>
       <c r="H203" t="s">
         <v>669</v>
       </c>
       <c r="I203" t="s">
-        <v>675</v>
+        <v>674</v>
+      </c>
+      <c r="K203">
+        <v>188.4816666666667</v>
+      </c>
+      <c r="L203">
+        <v>678534</v>
       </c>
       <c r="M203" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="Q203" t="s">
         <v>675</v>
@@ -10036,19 +10036,19 @@
         <v>24</v>
       </c>
       <c r="D204" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="E204" t="s">
-        <v>253</v>
+        <v>405</v>
       </c>
       <c r="F204" t="s">
         <v>614</v>
       </c>
       <c r="G204" t="s">
-        <v>617</v>
+        <v>636</v>
       </c>
       <c r="H204" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="I204" t="s">
         <v>675</v>
@@ -10334,7 +10334,7 @@
         <v>24</v>
       </c>
       <c r="D212" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E212" t="s">
         <v>411</v>
@@ -10369,7 +10369,7 @@
         <v>24</v>
       </c>
       <c r="D213" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E213" t="s">
         <v>412</v>
@@ -10431,7 +10431,7 @@
         <v>138.5375</v>
       </c>
       <c r="L214">
-        <v>498735.0000000001</v>
+        <v>498735</v>
       </c>
       <c r="M214" t="s">
         <v>682</v>
@@ -10562,7 +10562,7 @@
         <v>24</v>
       </c>
       <c r="D218" t="s">
-        <v>191</v>
+        <v>89</v>
       </c>
       <c r="E218" t="s">
         <v>415</v>
@@ -10571,7 +10571,7 @@
         <v>614</v>
       </c>
       <c r="G218" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="H218" t="s">
         <v>670</v>
@@ -10583,10 +10583,7 @@
         <v>678</v>
       </c>
       <c r="Q218" t="s">
-        <v>674</v>
-      </c>
-      <c r="R218">
-        <v>26020</v>
+        <v>675</v>
       </c>
     </row>
     <row r="219" spans="1:18">
@@ -10600,7 +10597,7 @@
         <v>24</v>
       </c>
       <c r="D219" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E219" t="s">
         <v>416</v>
@@ -10609,25 +10606,22 @@
         <v>614</v>
       </c>
       <c r="G219" t="s">
-        <v>630</v>
+        <v>621</v>
       </c>
       <c r="H219" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="I219" t="s">
-        <v>674</v>
-      </c>
-      <c r="K219">
-        <v>152.2927777777778</v>
-      </c>
-      <c r="L219">
-        <v>548254</v>
+        <v>675</v>
       </c>
       <c r="M219" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="Q219" t="s">
-        <v>675</v>
+        <v>674</v>
+      </c>
+      <c r="R219">
+        <v>26020</v>
       </c>
     </row>
     <row r="220" spans="1:18">
@@ -10641,7 +10635,7 @@
         <v>24</v>
       </c>
       <c r="D220" t="s">
-        <v>54</v>
+        <v>192</v>
       </c>
       <c r="E220" t="s">
         <v>417</v>
@@ -10650,7 +10644,7 @@
         <v>614</v>
       </c>
       <c r="G220" t="s">
-        <v>625</v>
+        <v>630</v>
       </c>
       <c r="H220" t="s">
         <v>669</v>
@@ -10659,13 +10653,13 @@
         <v>674</v>
       </c>
       <c r="K220">
-        <v>188.5294444444444</v>
+        <v>152.2927777777778</v>
       </c>
       <c r="L220">
-        <v>678706</v>
+        <v>548254</v>
       </c>
       <c r="M220" t="s">
-        <v>677</v>
+        <v>680</v>
       </c>
       <c r="Q220" t="s">
         <v>675</v>
@@ -10682,7 +10676,7 @@
         <v>24</v>
       </c>
       <c r="D221" t="s">
-        <v>89</v>
+        <v>54</v>
       </c>
       <c r="E221" t="s">
         <v>418</v>
@@ -10691,16 +10685,22 @@
         <v>614</v>
       </c>
       <c r="G221" t="s">
-        <v>617</v>
+        <v>625</v>
       </c>
       <c r="H221" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="I221" t="s">
-        <v>675</v>
+        <v>674</v>
+      </c>
+      <c r="K221">
+        <v>188.5294444444444</v>
+      </c>
+      <c r="L221">
+        <v>678706</v>
       </c>
       <c r="M221" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="Q221" t="s">
         <v>675</v>
@@ -10898,7 +10898,7 @@
         <v>24</v>
       </c>
       <c r="D227" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E227" t="s">
         <v>269</v>
@@ -11395,7 +11395,7 @@
         <v>24</v>
       </c>
       <c r="D240" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E240" t="s">
         <v>433</v>
@@ -11570,7 +11570,7 @@
         <v>24</v>
       </c>
       <c r="D245" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E245" t="s">
         <v>437</v>
@@ -11646,7 +11646,7 @@
         <v>24</v>
       </c>
       <c r="D247" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E247" t="s">
         <v>438</v>
@@ -11950,7 +11950,7 @@
         <v>24</v>
       </c>
       <c r="D255" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E255" t="s">
         <v>295</v>
@@ -12055,7 +12055,7 @@
         <v>24</v>
       </c>
       <c r="D258" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="E258" t="s">
         <v>296</v>
@@ -12064,10 +12064,10 @@
         <v>614</v>
       </c>
       <c r="G258" t="s">
-        <v>617</v>
+        <v>636</v>
       </c>
       <c r="H258" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="I258" t="s">
         <v>675</v>
@@ -12090,19 +12090,19 @@
         <v>24</v>
       </c>
       <c r="D259" t="s">
-        <v>42</v>
+        <v>143</v>
       </c>
       <c r="E259" t="s">
-        <v>448</v>
+        <v>297</v>
       </c>
       <c r="F259" t="s">
         <v>614</v>
       </c>
       <c r="G259" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="H259" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="I259" t="s">
         <v>675</v>
@@ -12125,19 +12125,19 @@
         <v>24</v>
       </c>
       <c r="D260" t="s">
-        <v>126</v>
+        <v>42</v>
       </c>
       <c r="E260" t="s">
-        <v>299</v>
+        <v>448</v>
       </c>
       <c r="F260" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="G260" t="s">
-        <v>641</v>
+        <v>621</v>
       </c>
       <c r="H260" t="s">
-        <v>669</v>
+        <v>672</v>
       </c>
       <c r="I260" t="s">
         <v>675</v>
@@ -12160,16 +12160,16 @@
         <v>24</v>
       </c>
       <c r="D261" t="s">
-        <v>71</v>
+        <v>127</v>
       </c>
       <c r="E261" t="s">
-        <v>449</v>
+        <v>300</v>
       </c>
       <c r="F261" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="G261" t="s">
-        <v>634</v>
+        <v>641</v>
       </c>
       <c r="H261" t="s">
         <v>669</v>
@@ -12195,19 +12195,19 @@
         <v>24</v>
       </c>
       <c r="D262" t="s">
-        <v>132</v>
+        <v>71</v>
       </c>
       <c r="E262" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F262" t="s">
         <v>614</v>
       </c>
       <c r="G262" t="s">
-        <v>630</v>
+        <v>634</v>
       </c>
       <c r="H262" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="I262" t="s">
         <v>675</v>
@@ -12230,10 +12230,10 @@
         <v>24</v>
       </c>
       <c r="D263" t="s">
-        <v>66</v>
+        <v>132</v>
       </c>
       <c r="E263" t="s">
-        <v>301</v>
+        <v>450</v>
       </c>
       <c r="F263" t="s">
         <v>614</v>
@@ -12242,7 +12242,7 @@
         <v>630</v>
       </c>
       <c r="H263" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="I263" t="s">
         <v>675</v>
@@ -12464,19 +12464,19 @@
         <v>24</v>
       </c>
       <c r="D269" t="s">
-        <v>107</v>
+        <v>66</v>
       </c>
       <c r="E269" t="s">
-        <v>455</v>
+        <v>306</v>
       </c>
       <c r="F269" t="s">
         <v>614</v>
       </c>
       <c r="G269" t="s">
-        <v>646</v>
+        <v>630</v>
       </c>
       <c r="H269" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="I269" t="s">
         <v>675</v>
@@ -12499,19 +12499,19 @@
         <v>24</v>
       </c>
       <c r="D270" t="s">
-        <v>161</v>
+        <v>107</v>
       </c>
       <c r="E270" t="s">
-        <v>306</v>
+        <v>455</v>
       </c>
       <c r="F270" t="s">
         <v>614</v>
       </c>
       <c r="G270" t="s">
-        <v>621</v>
+        <v>646</v>
       </c>
       <c r="H270" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="I270" t="s">
         <v>675</v>
@@ -12534,10 +12534,10 @@
         <v>24</v>
       </c>
       <c r="D271" t="s">
-        <v>91</v>
+        <v>161</v>
       </c>
       <c r="E271" t="s">
-        <v>456</v>
+        <v>307</v>
       </c>
       <c r="F271" t="s">
         <v>614</v>
@@ -12546,19 +12546,13 @@
         <v>621</v>
       </c>
       <c r="H271" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="I271" t="s">
-        <v>674</v>
-      </c>
-      <c r="K271">
-        <v>160.4947222222222</v>
-      </c>
-      <c r="L271">
-        <v>577781</v>
+        <v>675</v>
       </c>
       <c r="M271" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="Q271" t="s">
         <v>675</v>
@@ -12575,25 +12569,31 @@
         <v>24</v>
       </c>
       <c r="D272" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="E272" t="s">
-        <v>307</v>
+        <v>456</v>
       </c>
       <c r="F272" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="G272" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="H272" t="s">
         <v>670</v>
       </c>
       <c r="I272" t="s">
-        <v>675</v>
+        <v>674</v>
+      </c>
+      <c r="K272">
+        <v>160.4947222222222</v>
+      </c>
+      <c r="L272">
+        <v>577781</v>
       </c>
       <c r="M272" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="Q272" t="s">
         <v>675</v>
@@ -12610,31 +12610,25 @@
         <v>24</v>
       </c>
       <c r="D273" t="s">
-        <v>198</v>
+        <v>118</v>
       </c>
       <c r="E273" t="s">
-        <v>457</v>
+        <v>308</v>
       </c>
       <c r="F273" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="G273" t="s">
-        <v>621</v>
+        <v>634</v>
       </c>
       <c r="H273" t="s">
         <v>670</v>
       </c>
       <c r="I273" t="s">
-        <v>674</v>
-      </c>
-      <c r="K273">
-        <v>183.4911111111111</v>
-      </c>
-      <c r="L273">
-        <v>660568</v>
+        <v>675</v>
       </c>
       <c r="M273" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="Q273" t="s">
         <v>675</v>
@@ -12651,25 +12645,31 @@
         <v>24</v>
       </c>
       <c r="D274" t="s">
-        <v>70</v>
+        <v>198</v>
       </c>
       <c r="E274" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F274" t="s">
         <v>614</v>
       </c>
       <c r="G274" t="s">
-        <v>648</v>
+        <v>621</v>
       </c>
       <c r="H274" t="s">
         <v>670</v>
       </c>
       <c r="I274" t="s">
-        <v>675</v>
+        <v>674</v>
+      </c>
+      <c r="K274">
+        <v>183.4911111111111</v>
+      </c>
+      <c r="L274">
+        <v>660568</v>
       </c>
       <c r="M274" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="Q274" t="s">
         <v>675</v>
@@ -12686,19 +12686,19 @@
         <v>24</v>
       </c>
       <c r="D275" t="s">
-        <v>152</v>
+        <v>70</v>
       </c>
       <c r="E275" t="s">
-        <v>310</v>
+        <v>458</v>
       </c>
       <c r="F275" t="s">
         <v>614</v>
       </c>
       <c r="G275" t="s">
-        <v>617</v>
+        <v>648</v>
       </c>
       <c r="H275" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="I275" t="s">
         <v>675</v>
@@ -12721,10 +12721,10 @@
         <v>24</v>
       </c>
       <c r="D276" t="s">
-        <v>199</v>
+        <v>152</v>
       </c>
       <c r="E276" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="F276" t="s">
         <v>614</v>
@@ -12756,31 +12756,25 @@
         <v>24</v>
       </c>
       <c r="D277" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E277" t="s">
-        <v>459</v>
+        <v>315</v>
       </c>
       <c r="F277" t="s">
         <v>614</v>
       </c>
       <c r="G277" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="H277" t="s">
         <v>669</v>
       </c>
       <c r="I277" t="s">
-        <v>674</v>
-      </c>
-      <c r="K277">
-        <v>169.5202777777778</v>
-      </c>
-      <c r="L277">
-        <v>610273</v>
+        <v>675</v>
       </c>
       <c r="M277" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="Q277" t="s">
         <v>675</v>
@@ -12797,16 +12791,16 @@
         <v>24</v>
       </c>
       <c r="D278" t="s">
-        <v>57</v>
+        <v>200</v>
       </c>
       <c r="E278" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="F278" t="s">
         <v>614</v>
       </c>
       <c r="G278" t="s">
-        <v>617</v>
+        <v>621</v>
       </c>
       <c r="H278" t="s">
         <v>669</v>
@@ -12815,13 +12809,13 @@
         <v>674</v>
       </c>
       <c r="K278">
-        <v>159.1452777777778</v>
+        <v>169.5202777777778</v>
       </c>
       <c r="L278">
-        <v>572923</v>
+        <v>610273</v>
       </c>
       <c r="M278" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="Q278" t="s">
         <v>675</v>
@@ -12838,25 +12832,31 @@
         <v>24</v>
       </c>
       <c r="D279" t="s">
-        <v>201</v>
+        <v>57</v>
       </c>
       <c r="E279" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="F279" t="s">
         <v>614</v>
       </c>
       <c r="G279" t="s">
-        <v>654</v>
+        <v>617</v>
       </c>
       <c r="H279" t="s">
         <v>669</v>
       </c>
       <c r="I279" t="s">
-        <v>675</v>
+        <v>674</v>
+      </c>
+      <c r="K279">
+        <v>159.1452777777778</v>
+      </c>
+      <c r="L279">
+        <v>572923</v>
       </c>
       <c r="M279" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="Q279" t="s">
         <v>675</v>
@@ -12873,31 +12873,25 @@
         <v>24</v>
       </c>
       <c r="D280" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="E280" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F280" t="s">
         <v>614</v>
       </c>
       <c r="G280" t="s">
-        <v>621</v>
+        <v>654</v>
       </c>
       <c r="H280" t="s">
         <v>669</v>
       </c>
       <c r="I280" t="s">
-        <v>674</v>
-      </c>
-      <c r="K280">
-        <v>185.7330555555556</v>
-      </c>
-      <c r="L280">
-        <v>668639</v>
+        <v>675</v>
       </c>
       <c r="M280" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="Q280" t="s">
         <v>675</v>
@@ -12914,25 +12908,31 @@
         <v>24</v>
       </c>
       <c r="D281" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="E281" t="s">
-        <v>317</v>
+        <v>462</v>
       </c>
       <c r="F281" t="s">
         <v>614</v>
       </c>
       <c r="G281" t="s">
-        <v>636</v>
+        <v>621</v>
       </c>
       <c r="H281" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="I281" t="s">
-        <v>675</v>
+        <v>674</v>
+      </c>
+      <c r="K281">
+        <v>185.7330555555556</v>
+      </c>
+      <c r="L281">
+        <v>668639</v>
       </c>
       <c r="M281" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="Q281" t="s">
         <v>675</v>
@@ -12949,31 +12949,25 @@
         <v>24</v>
       </c>
       <c r="D282" t="s">
-        <v>202</v>
+        <v>32</v>
       </c>
       <c r="E282" t="s">
-        <v>320</v>
+        <v>463</v>
       </c>
       <c r="F282" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="G282" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="H282" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="I282" t="s">
-        <v>674</v>
-      </c>
-      <c r="K282">
-        <v>159.9830555555556</v>
-      </c>
-      <c r="L282">
-        <v>575939</v>
+        <v>675</v>
       </c>
       <c r="M282" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="Q282" t="s">
         <v>675</v>
@@ -12990,25 +12984,31 @@
         <v>24</v>
       </c>
       <c r="D283" t="s">
-        <v>81</v>
+        <v>202</v>
       </c>
       <c r="E283" t="s">
-        <v>463</v>
+        <v>320</v>
       </c>
       <c r="F283" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="G283" t="s">
-        <v>632</v>
+        <v>621</v>
       </c>
       <c r="H283" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c r="I283" t="s">
-        <v>675</v>
+        <v>674</v>
+      </c>
+      <c r="K283">
+        <v>159.9830555555556</v>
+      </c>
+      <c r="L283">
+        <v>575939</v>
       </c>
       <c r="M283" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="Q283" t="s">
         <v>675</v>
@@ -13025,7 +13025,7 @@
         <v>24</v>
       </c>
       <c r="D284" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="E284" t="s">
         <v>464</v>
@@ -13034,7 +13034,7 @@
         <v>614</v>
       </c>
       <c r="G284" t="s">
-        <v>617</v>
+        <v>632</v>
       </c>
       <c r="H284" t="s">
         <v>669</v>
@@ -13060,10 +13060,10 @@
         <v>24</v>
       </c>
       <c r="D285" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="E285" t="s">
-        <v>321</v>
+        <v>465</v>
       </c>
       <c r="F285" t="s">
         <v>614</v>
@@ -13075,16 +13075,10 @@
         <v>669</v>
       </c>
       <c r="I285" t="s">
-        <v>674</v>
-      </c>
-      <c r="K285">
-        <v>187.2547222222222</v>
-      </c>
-      <c r="L285">
-        <v>674117</v>
+        <v>675</v>
       </c>
       <c r="M285" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="Q285" t="s">
         <v>675</v>
@@ -13101,25 +13095,31 @@
         <v>24</v>
       </c>
       <c r="D286" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E286" t="s">
-        <v>465</v>
+        <v>321</v>
       </c>
       <c r="F286" t="s">
         <v>614</v>
       </c>
       <c r="G286" t="s">
-        <v>638</v>
+        <v>617</v>
       </c>
       <c r="H286" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="I286" t="s">
-        <v>675</v>
+        <v>674</v>
+      </c>
+      <c r="K286">
+        <v>187.2547222222222</v>
+      </c>
+      <c r="L286">
+        <v>674117</v>
       </c>
       <c r="M286" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="Q286" t="s">
         <v>675</v>
@@ -13136,7 +13136,7 @@
         <v>24</v>
       </c>
       <c r="D287" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="E287" t="s">
         <v>466</v>
@@ -13145,10 +13145,10 @@
         <v>614</v>
       </c>
       <c r="G287" t="s">
-        <v>621</v>
+        <v>638</v>
       </c>
       <c r="H287" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="I287" t="s">
         <v>675</v>
@@ -13171,7 +13171,7 @@
         <v>24</v>
       </c>
       <c r="D288" t="s">
-        <v>93</v>
+        <v>134</v>
       </c>
       <c r="E288" t="s">
         <v>467</v>
@@ -13180,10 +13180,10 @@
         <v>614</v>
       </c>
       <c r="G288" t="s">
-        <v>638</v>
+        <v>621</v>
       </c>
       <c r="H288" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c r="I288" t="s">
         <v>675</v>
@@ -13206,7 +13206,7 @@
         <v>24</v>
       </c>
       <c r="D289" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="E289" t="s">
         <v>468</v>
@@ -13215,22 +13215,16 @@
         <v>614</v>
       </c>
       <c r="G289" t="s">
-        <v>620</v>
+        <v>638</v>
       </c>
       <c r="H289" t="s">
         <v>669</v>
       </c>
       <c r="I289" t="s">
-        <v>674</v>
-      </c>
-      <c r="K289">
-        <v>185.8447222222222</v>
-      </c>
-      <c r="L289">
-        <v>669041</v>
+        <v>675</v>
       </c>
       <c r="M289" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="Q289" t="s">
         <v>675</v>
@@ -13247,31 +13241,31 @@
         <v>24</v>
       </c>
       <c r="D290" t="s">
-        <v>203</v>
+        <v>34</v>
       </c>
       <c r="E290" t="s">
-        <v>328</v>
+        <v>469</v>
       </c>
       <c r="F290" t="s">
         <v>614</v>
       </c>
       <c r="G290" t="s">
-        <v>644</v>
+        <v>620</v>
       </c>
       <c r="H290" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="I290" t="s">
         <v>674</v>
       </c>
       <c r="K290">
-        <v>178.4855555555555</v>
+        <v>185.8447222222222</v>
       </c>
       <c r="L290">
-        <v>642548</v>
+        <v>669041</v>
       </c>
       <c r="M290" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="Q290" t="s">
         <v>675</v>
@@ -13288,31 +13282,31 @@
         <v>24</v>
       </c>
       <c r="D291" t="s">
-        <v>79</v>
+        <v>203</v>
       </c>
       <c r="E291" t="s">
-        <v>469</v>
+        <v>328</v>
       </c>
       <c r="F291" t="s">
         <v>614</v>
       </c>
       <c r="G291" t="s">
-        <v>621</v>
+        <v>644</v>
       </c>
       <c r="H291" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="I291" t="s">
         <v>674</v>
       </c>
       <c r="K291">
-        <v>187.4063888888889</v>
+        <v>178.4855555555555</v>
       </c>
       <c r="L291">
-        <v>674663</v>
+        <v>642548</v>
       </c>
       <c r="M291" t="s">
-        <v>677</v>
+        <v>681</v>
       </c>
       <c r="Q291" t="s">
         <v>675</v>
@@ -13329,25 +13323,31 @@
         <v>24</v>
       </c>
       <c r="D292" t="s">
-        <v>139</v>
+        <v>79</v>
       </c>
       <c r="E292" t="s">
         <v>470</v>
       </c>
       <c r="F292" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="G292" t="s">
-        <v>618</v>
+        <v>621</v>
       </c>
       <c r="H292" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="I292" t="s">
-        <v>675</v>
+        <v>674</v>
+      </c>
+      <c r="K292">
+        <v>187.4063888888889</v>
+      </c>
+      <c r="L292">
+        <v>674663</v>
       </c>
       <c r="M292" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="Q292" t="s">
         <v>675</v>
@@ -13364,31 +13364,25 @@
         <v>24</v>
       </c>
       <c r="D293" t="s">
-        <v>204</v>
+        <v>139</v>
       </c>
       <c r="E293" t="s">
         <v>471</v>
       </c>
       <c r="F293" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="G293" t="s">
-        <v>625</v>
+        <v>618</v>
       </c>
       <c r="H293" t="s">
         <v>669</v>
       </c>
       <c r="I293" t="s">
-        <v>674</v>
-      </c>
-      <c r="K293">
-        <v>178.2983333333333</v>
-      </c>
-      <c r="L293">
-        <v>641874</v>
+        <v>675</v>
       </c>
       <c r="M293" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="Q293" t="s">
         <v>675</v>
@@ -13405,7 +13399,7 @@
         <v>24</v>
       </c>
       <c r="D294" t="s">
-        <v>62</v>
+        <v>204</v>
       </c>
       <c r="E294" t="s">
         <v>472</v>
@@ -13414,16 +13408,22 @@
         <v>614</v>
       </c>
       <c r="G294" t="s">
-        <v>621</v>
+        <v>625</v>
       </c>
       <c r="H294" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="I294" t="s">
-        <v>675</v>
+        <v>674</v>
+      </c>
+      <c r="K294">
+        <v>178.2983333333333</v>
+      </c>
+      <c r="L294">
+        <v>641874</v>
       </c>
       <c r="M294" t="s">
-        <v>678</v>
+        <v>681</v>
       </c>
       <c r="Q294" t="s">
         <v>675</v>
@@ -13440,7 +13440,7 @@
         <v>24</v>
       </c>
       <c r="D295" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="E295" t="s">
         <v>473</v>
@@ -13449,22 +13449,16 @@
         <v>614</v>
       </c>
       <c r="G295" t="s">
-        <v>617</v>
+        <v>621</v>
       </c>
       <c r="H295" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="I295" t="s">
-        <v>674</v>
-      </c>
-      <c r="K295">
-        <v>187.2677777777778</v>
-      </c>
-      <c r="L295">
-        <v>674164</v>
+        <v>675</v>
       </c>
       <c r="M295" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="Q295" t="s">
         <v>675</v>
@@ -13481,25 +13475,31 @@
         <v>24</v>
       </c>
       <c r="D296" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="E296" t="s">
-        <v>329</v>
+        <v>474</v>
       </c>
       <c r="F296" t="s">
         <v>614</v>
       </c>
       <c r="G296" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="H296" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="I296" t="s">
-        <v>675</v>
+        <v>674</v>
+      </c>
+      <c r="K296">
+        <v>187.2677777777778</v>
+      </c>
+      <c r="L296">
+        <v>674164</v>
       </c>
       <c r="M296" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="Q296" t="s">
         <v>675</v>
@@ -13516,10 +13516,10 @@
         <v>24</v>
       </c>
       <c r="D297" t="s">
-        <v>147</v>
+        <v>86</v>
       </c>
       <c r="E297" t="s">
-        <v>474</v>
+        <v>329</v>
       </c>
       <c r="F297" t="s">
         <v>614</v>
@@ -13528,19 +13528,13 @@
         <v>621</v>
       </c>
       <c r="H297" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c r="I297" t="s">
-        <v>674</v>
-      </c>
-      <c r="K297">
-        <v>143.0308333333334</v>
-      </c>
-      <c r="L297">
-        <v>514911.0000000001</v>
+        <v>675</v>
       </c>
       <c r="M297" t="s">
-        <v>683</v>
+        <v>678</v>
       </c>
       <c r="Q297" t="s">
         <v>675</v>
@@ -13557,7 +13551,7 @@
         <v>24</v>
       </c>
       <c r="D298" t="s">
-        <v>28</v>
+        <v>147</v>
       </c>
       <c r="E298" t="s">
         <v>475</v>
@@ -13566,16 +13560,22 @@
         <v>614</v>
       </c>
       <c r="G298" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="H298" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="I298" t="s">
-        <v>675</v>
+        <v>674</v>
+      </c>
+      <c r="K298">
+        <v>143.0308333333333</v>
+      </c>
+      <c r="L298">
+        <v>514911</v>
       </c>
       <c r="M298" t="s">
-        <v>678</v>
+        <v>683</v>
       </c>
       <c r="Q298" t="s">
         <v>675</v>
@@ -13592,7 +13592,7 @@
         <v>24</v>
       </c>
       <c r="D299" t="s">
-        <v>85</v>
+        <v>28</v>
       </c>
       <c r="E299" t="s">
         <v>476</v>
@@ -13601,22 +13601,16 @@
         <v>614</v>
       </c>
       <c r="G299" t="s">
-        <v>621</v>
+        <v>634</v>
       </c>
       <c r="H299" t="s">
         <v>670</v>
       </c>
       <c r="I299" t="s">
-        <v>674</v>
-      </c>
-      <c r="K299">
-        <v>185.2544444444444</v>
-      </c>
-      <c r="L299">
-        <v>666916</v>
+        <v>675</v>
       </c>
       <c r="M299" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="Q299" t="s">
         <v>675</v>
@@ -13633,25 +13627,31 @@
         <v>24</v>
       </c>
       <c r="D300" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="E300" t="s">
         <v>477</v>
       </c>
       <c r="F300" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="G300" t="s">
-        <v>638</v>
+        <v>621</v>
       </c>
       <c r="H300" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="I300" t="s">
-        <v>675</v>
+        <v>674</v>
+      </c>
+      <c r="K300">
+        <v>185.2544444444444</v>
+      </c>
+      <c r="L300">
+        <v>666916</v>
       </c>
       <c r="M300" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="Q300" t="s">
         <v>675</v>
@@ -13668,19 +13668,19 @@
         <v>24</v>
       </c>
       <c r="D301" t="s">
-        <v>164</v>
+        <v>111</v>
       </c>
       <c r="E301" t="s">
-        <v>337</v>
+        <v>478</v>
       </c>
       <c r="F301" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="G301" t="s">
-        <v>625</v>
+        <v>638</v>
       </c>
       <c r="H301" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="I301" t="s">
         <v>675</v>
@@ -13703,31 +13703,25 @@
         <v>24</v>
       </c>
       <c r="D302" t="s">
-        <v>92</v>
+        <v>164</v>
       </c>
       <c r="E302" t="s">
-        <v>478</v>
+        <v>337</v>
       </c>
       <c r="F302" t="s">
         <v>614</v>
       </c>
       <c r="G302" t="s">
-        <v>636</v>
+        <v>625</v>
       </c>
       <c r="H302" t="s">
         <v>670</v>
       </c>
       <c r="I302" t="s">
-        <v>674</v>
-      </c>
-      <c r="K302">
-        <v>175.2175</v>
-      </c>
-      <c r="L302">
-        <v>630783</v>
+        <v>675</v>
       </c>
       <c r="M302" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="Q302" t="s">
         <v>675</v>
@@ -13744,25 +13738,31 @@
         <v>24</v>
       </c>
       <c r="D303" t="s">
-        <v>162</v>
+        <v>92</v>
       </c>
       <c r="E303" t="s">
-        <v>340</v>
+        <v>479</v>
       </c>
       <c r="F303" t="s">
         <v>614</v>
       </c>
       <c r="G303" t="s">
-        <v>621</v>
+        <v>636</v>
       </c>
       <c r="H303" t="s">
         <v>670</v>
       </c>
       <c r="I303" t="s">
-        <v>675</v>
+        <v>674</v>
+      </c>
+      <c r="K303">
+        <v>175.2175</v>
+      </c>
+      <c r="L303">
+        <v>630783</v>
       </c>
       <c r="M303" t="s">
-        <v>678</v>
+        <v>681</v>
       </c>
       <c r="Q303" t="s">
         <v>675</v>
@@ -13779,19 +13779,19 @@
         <v>24</v>
       </c>
       <c r="D304" t="s">
-        <v>32</v>
+        <v>162</v>
       </c>
       <c r="E304" t="s">
-        <v>479</v>
+        <v>340</v>
       </c>
       <c r="F304" t="s">
         <v>614</v>
       </c>
       <c r="G304" t="s">
-        <v>617</v>
+        <v>621</v>
       </c>
       <c r="H304" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="I304" t="s">
         <v>675</v>
@@ -13890,7 +13890,7 @@
         <v>24</v>
       </c>
       <c r="D307" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E307" t="s">
         <v>343</v>
@@ -14696,7 +14696,7 @@
         <v>24</v>
       </c>
       <c r="D329" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E329" t="s">
         <v>498</v>
@@ -14766,7 +14766,7 @@
         <v>25</v>
       </c>
       <c r="D331" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E331" t="s">
         <v>359</v>
@@ -14877,7 +14877,7 @@
         <v>25</v>
       </c>
       <c r="D334" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E334" t="s">
         <v>361</v>
@@ -14953,7 +14953,7 @@
         <v>25</v>
       </c>
       <c r="D336" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E336" t="s">
         <v>363</v>
@@ -15175,7 +15175,7 @@
         <v>25</v>
       </c>
       <c r="D342" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E342" t="s">
         <v>228</v>
@@ -15596,7 +15596,7 @@
         <v>25</v>
       </c>
       <c r="D353" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E353" t="s">
         <v>239</v>
@@ -15631,7 +15631,7 @@
         <v>25</v>
       </c>
       <c r="D354" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E354" t="s">
         <v>506</v>
@@ -15845,7 +15845,7 @@
         <v>135.3666666666667</v>
       </c>
       <c r="L359">
-        <v>487320.0000000001</v>
+        <v>487320</v>
       </c>
       <c r="M359" t="s">
         <v>682</v>
@@ -16347,7 +16347,7 @@
         <v>25</v>
       </c>
       <c r="D373" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E373" t="s">
         <v>400</v>
@@ -16473,7 +16473,7 @@
         <v>143.2347222222222</v>
       </c>
       <c r="L376">
-        <v>515645.0000000001</v>
+        <v>515645</v>
       </c>
       <c r="M376" t="s">
         <v>683</v>
@@ -16572,7 +16572,7 @@
         <v>68</v>
       </c>
       <c r="E379" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="F379" t="s">
         <v>615</v>
@@ -16929,7 +16929,7 @@
         <v>132.9877777777778</v>
       </c>
       <c r="L388">
-        <v>478756.0000000001</v>
+        <v>478756</v>
       </c>
       <c r="M388" t="s">
         <v>682</v>
@@ -16970,7 +16970,7 @@
         <v>132.9908333333333</v>
       </c>
       <c r="L389">
-        <v>478767.0000000001</v>
+        <v>478767</v>
       </c>
       <c r="M389" t="s">
         <v>682</v>
@@ -16990,7 +16990,7 @@
         <v>25</v>
       </c>
       <c r="D390" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E390" t="s">
         <v>528</v>
@@ -17195,7 +17195,7 @@
         <v>25</v>
       </c>
       <c r="D395" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E395" t="s">
         <v>531</v>
@@ -17411,7 +17411,7 @@
         <v>25</v>
       </c>
       <c r="D401" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E401" t="s">
         <v>269</v>
@@ -17759,7 +17759,7 @@
         <v>25</v>
       </c>
       <c r="D410" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E410" t="s">
         <v>280</v>
@@ -17996,16 +17996,10 @@
         <v>671</v>
       </c>
       <c r="I416" t="s">
-        <v>674</v>
-      </c>
-      <c r="K416">
-        <v>163.4244444444444</v>
-      </c>
-      <c r="L416">
-        <v>588328</v>
+        <v>675</v>
       </c>
       <c r="M416" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="Q416" t="s">
         <v>674</v>
@@ -18148,7 +18142,7 @@
         <v>25</v>
       </c>
       <c r="D420" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E420" t="s">
         <v>544</v>
@@ -18172,7 +18166,7 @@
         <v>674</v>
       </c>
       <c r="R420">
-        <v>969.0000000000001</v>
+        <v>969</v>
       </c>
     </row>
     <row r="421" spans="1:18">
@@ -18490,7 +18484,7 @@
         <v>25</v>
       </c>
       <c r="D429" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E429" t="s">
         <v>550</v>
@@ -18642,10 +18636,10 @@
         <v>25</v>
       </c>
       <c r="D433" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E433" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="F433" t="s">
         <v>615</v>
@@ -18873,7 +18867,7 @@
         <v>189</v>
       </c>
       <c r="E439" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="F439" t="s">
         <v>614</v>
@@ -18914,7 +18908,7 @@
         <v>156</v>
       </c>
       <c r="E440" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F440" t="s">
         <v>614</v>
@@ -19002,16 +18996,10 @@
         <v>670</v>
       </c>
       <c r="I442" t="s">
-        <v>674</v>
-      </c>
-      <c r="K442">
-        <v>158.8377777777778</v>
-      </c>
-      <c r="L442">
-        <v>571816</v>
+        <v>675</v>
       </c>
       <c r="M442" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="Q442" t="s">
         <v>675</v>
@@ -19107,7 +19095,7 @@
         <v>87</v>
       </c>
       <c r="E445" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="F445" t="s">
         <v>614</v>
@@ -19142,7 +19130,7 @@
         <v>155</v>
       </c>
       <c r="E446" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="F446" t="s">
         <v>614</v>
@@ -19183,7 +19171,7 @@
         <v>132</v>
       </c>
       <c r="E447" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="F447" t="s">
         <v>614</v>
@@ -19335,7 +19323,7 @@
         <v>207</v>
       </c>
       <c r="E451" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="F451" t="s">
         <v>614</v>
@@ -19721,7 +19709,7 @@
         <v>167</v>
       </c>
       <c r="E461" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="F461" t="s">
         <v>614</v>
@@ -19794,7 +19782,7 @@
         <v>25</v>
       </c>
       <c r="D463" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E463" t="s">
         <v>326</v>
@@ -19835,7 +19823,7 @@
         <v>25</v>
       </c>
       <c r="D464" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E464" t="s">
         <v>567</v>
@@ -19914,7 +19902,7 @@
         <v>134</v>
       </c>
       <c r="E466" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="F466" t="s">
         <v>614</v>
@@ -20031,7 +20019,7 @@
         <v>170</v>
       </c>
       <c r="E469" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="F469" t="s">
         <v>614</v>
@@ -20101,7 +20089,7 @@
         <v>115</v>
       </c>
       <c r="E471" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="F471" t="s">
         <v>614</v>
@@ -20177,7 +20165,7 @@
         <v>141</v>
       </c>
       <c r="E473" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="F473" t="s">
         <v>614</v>
@@ -20285,7 +20273,7 @@
         <v>25</v>
       </c>
       <c r="D476" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E476" t="s">
         <v>572</v>
@@ -20566,7 +20554,7 @@
         <v>25</v>
       </c>
       <c r="D483" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E483" t="s">
         <v>484</v>
@@ -20581,16 +20569,10 @@
         <v>669</v>
       </c>
       <c r="I483" t="s">
-        <v>674</v>
-      </c>
-      <c r="K483">
-        <v>181.8886111111111</v>
-      </c>
-      <c r="L483">
-        <v>654799</v>
+        <v>675</v>
       </c>
       <c r="M483" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="Q483" t="s">
         <v>675</v>
@@ -20695,16 +20677,10 @@
         <v>669</v>
       </c>
       <c r="I486" t="s">
-        <v>674</v>
-      </c>
-      <c r="K486">
-        <v>160.7108333333333</v>
-      </c>
-      <c r="L486">
-        <v>578559</v>
+        <v>675</v>
       </c>
       <c r="M486" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="Q486" t="s">
         <v>675</v>
@@ -20853,7 +20829,7 @@
         <v>135.3666666666667</v>
       </c>
       <c r="L490">
-        <v>487320.0000000001</v>
+        <v>487320</v>
       </c>
       <c r="M490" t="s">
         <v>682</v>
@@ -20873,16 +20849,16 @@
         <v>25</v>
       </c>
       <c r="D491" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="E491" t="s">
-        <v>488</v>
+        <v>577</v>
       </c>
       <c r="F491" t="s">
         <v>614</v>
       </c>
       <c r="G491" t="s">
-        <v>621</v>
+        <v>626</v>
       </c>
       <c r="H491" t="s">
         <v>669</v>
@@ -20908,10 +20884,10 @@
         <v>25</v>
       </c>
       <c r="D492" t="s">
-        <v>143</v>
+        <v>60</v>
       </c>
       <c r="E492" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="F492" t="s">
         <v>614</v>
@@ -20920,7 +20896,7 @@
         <v>621</v>
       </c>
       <c r="H492" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="I492" t="s">
         <v>675</v>
@@ -20943,19 +20919,19 @@
         <v>25</v>
       </c>
       <c r="D493" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="E493" t="s">
-        <v>350</v>
+        <v>489</v>
       </c>
       <c r="F493" t="s">
         <v>614</v>
       </c>
       <c r="G493" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="H493" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="I493" t="s">
         <v>675</v>
@@ -20978,31 +20954,25 @@
         <v>25</v>
       </c>
       <c r="D494" t="s">
-        <v>56</v>
+        <v>164</v>
       </c>
       <c r="E494" t="s">
-        <v>577</v>
+        <v>350</v>
       </c>
       <c r="F494" t="s">
         <v>614</v>
       </c>
       <c r="G494" t="s">
-        <v>620</v>
+        <v>625</v>
       </c>
       <c r="H494" t="s">
         <v>670</v>
       </c>
       <c r="I494" t="s">
-        <v>674</v>
-      </c>
-      <c r="K494">
-        <v>181.4666666666667</v>
-      </c>
-      <c r="L494">
-        <v>653280</v>
+        <v>675</v>
       </c>
       <c r="M494" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="Q494" t="s">
         <v>675</v>
@@ -21019,7 +20989,7 @@
         <v>25</v>
       </c>
       <c r="D495" t="s">
-        <v>204</v>
+        <v>56</v>
       </c>
       <c r="E495" t="s">
         <v>578</v>
@@ -21028,19 +20998,19 @@
         <v>614</v>
       </c>
       <c r="G495" t="s">
-        <v>659</v>
+        <v>620</v>
       </c>
       <c r="H495" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="I495" t="s">
         <v>674</v>
       </c>
       <c r="K495">
-        <v>183.1002777777778</v>
+        <v>181.4666666666667</v>
       </c>
       <c r="L495">
-        <v>659161</v>
+        <v>653280</v>
       </c>
       <c r="M495" t="s">
         <v>677</v>
@@ -21060,7 +21030,7 @@
         <v>25</v>
       </c>
       <c r="D496" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="E496" t="s">
         <v>579</v>
@@ -21069,7 +21039,7 @@
         <v>614</v>
       </c>
       <c r="G496" t="s">
-        <v>625</v>
+        <v>659</v>
       </c>
       <c r="H496" t="s">
         <v>672</v>
@@ -21078,13 +21048,13 @@
         <v>674</v>
       </c>
       <c r="K496">
-        <v>162.8833333333333</v>
+        <v>183.1002777777778</v>
       </c>
       <c r="L496">
-        <v>586380</v>
+        <v>659161</v>
       </c>
       <c r="M496" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="Q496" t="s">
         <v>675</v>
@@ -21101,7 +21071,7 @@
         <v>25</v>
       </c>
       <c r="D497" t="s">
-        <v>34</v>
+        <v>214</v>
       </c>
       <c r="E497" t="s">
         <v>580</v>
@@ -21110,19 +21080,19 @@
         <v>614</v>
       </c>
       <c r="G497" t="s">
-        <v>621</v>
+        <v>625</v>
       </c>
       <c r="H497" t="s">
-        <v>669</v>
+        <v>672</v>
       </c>
       <c r="I497" t="s">
         <v>674</v>
       </c>
       <c r="K497">
-        <v>169.7333333333333</v>
+        <v>162.8833333333333</v>
       </c>
       <c r="L497">
-        <v>611040</v>
+        <v>586380</v>
       </c>
       <c r="M497" t="s">
         <v>679</v>
@@ -21142,7 +21112,7 @@
         <v>25</v>
       </c>
       <c r="D498" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E498" t="s">
         <v>581</v>
@@ -21151,16 +21121,22 @@
         <v>614</v>
       </c>
       <c r="G498" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
       <c r="H498" t="s">
         <v>669</v>
       </c>
       <c r="I498" t="s">
-        <v>675</v>
+        <v>674</v>
+      </c>
+      <c r="K498">
+        <v>169.7333333333333</v>
+      </c>
+      <c r="L498">
+        <v>611040</v>
       </c>
       <c r="M498" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="Q498" t="s">
         <v>675</v>
@@ -21715,7 +21691,7 @@
         <v>26</v>
       </c>
       <c r="D513" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E513" t="s">
         <v>590</v>
@@ -21750,7 +21726,7 @@
         <v>26</v>
       </c>
       <c r="D514" t="s">
-        <v>149</v>
+        <v>74</v>
       </c>
       <c r="E514" t="s">
         <v>591</v>
@@ -21759,7 +21735,7 @@
         <v>614</v>
       </c>
       <c r="G514" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="H514" t="s">
         <v>670</v>
@@ -21785,31 +21761,25 @@
         <v>26</v>
       </c>
       <c r="D515" t="s">
-        <v>70</v>
+        <v>149</v>
       </c>
       <c r="E515" t="s">
-        <v>257</v>
+        <v>592</v>
       </c>
       <c r="F515" t="s">
         <v>614</v>
       </c>
       <c r="G515" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
       <c r="H515" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="I515" t="s">
-        <v>674</v>
-      </c>
-      <c r="K515">
-        <v>173.4772222222222</v>
-      </c>
-      <c r="L515">
-        <v>624518</v>
+        <v>675</v>
       </c>
       <c r="M515" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="Q515" t="s">
         <v>675</v>
@@ -21826,16 +21796,16 @@
         <v>26</v>
       </c>
       <c r="D516" t="s">
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="E516" t="s">
-        <v>527</v>
+        <v>257</v>
       </c>
       <c r="F516" t="s">
         <v>614</v>
       </c>
       <c r="G516" t="s">
-        <v>620</v>
+        <v>626</v>
       </c>
       <c r="H516" t="s">
         <v>672</v>
@@ -21844,13 +21814,13 @@
         <v>674</v>
       </c>
       <c r="K516">
-        <v>138.3</v>
+        <v>173.4772222222222</v>
       </c>
       <c r="L516">
-        <v>497880.0000000001</v>
+        <v>624518</v>
       </c>
       <c r="M516" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="Q516" t="s">
         <v>675</v>
@@ -21867,25 +21837,31 @@
         <v>26</v>
       </c>
       <c r="D517" t="s">
-        <v>122</v>
+        <v>42</v>
       </c>
       <c r="E517" t="s">
-        <v>592</v>
+        <v>527</v>
       </c>
       <c r="F517" t="s">
         <v>614</v>
       </c>
       <c r="G517" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="H517" t="s">
         <v>672</v>
       </c>
       <c r="I517" t="s">
-        <v>675</v>
+        <v>674</v>
+      </c>
+      <c r="K517">
+        <v>138.3</v>
+      </c>
+      <c r="L517">
+        <v>497880</v>
       </c>
       <c r="M517" t="s">
-        <v>678</v>
+        <v>682</v>
       </c>
       <c r="Q517" t="s">
         <v>675</v>
@@ -21902,7 +21878,7 @@
         <v>26</v>
       </c>
       <c r="D518" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="E518" t="s">
         <v>593</v>
@@ -21914,7 +21890,7 @@
         <v>621</v>
       </c>
       <c r="H518" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="I518" t="s">
         <v>675</v>
@@ -21937,7 +21913,7 @@
         <v>26</v>
       </c>
       <c r="D519" t="s">
-        <v>65</v>
+        <v>111</v>
       </c>
       <c r="E519" t="s">
         <v>594</v>
@@ -21946,22 +21922,16 @@
         <v>614</v>
       </c>
       <c r="G519" t="s">
-        <v>630</v>
+        <v>621</v>
       </c>
       <c r="H519" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="I519" t="s">
-        <v>674</v>
-      </c>
-      <c r="K519">
-        <v>158.7538888888889</v>
-      </c>
-      <c r="L519">
-        <v>571514</v>
+        <v>675</v>
       </c>
       <c r="M519" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="Q519" t="s">
         <v>675</v>
@@ -21978,31 +21948,31 @@
         <v>26</v>
       </c>
       <c r="D520" t="s">
-        <v>101</v>
+        <v>63</v>
       </c>
       <c r="E520" t="s">
-        <v>276</v>
+        <v>595</v>
       </c>
       <c r="F520" t="s">
         <v>614</v>
       </c>
       <c r="G520" t="s">
-        <v>626</v>
+        <v>630</v>
       </c>
       <c r="H520" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="I520" t="s">
         <v>674</v>
       </c>
       <c r="K520">
-        <v>180.4405555555556</v>
+        <v>158.7538888888889</v>
       </c>
       <c r="L520">
-        <v>649586</v>
+        <v>571514</v>
       </c>
       <c r="M520" t="s">
-        <v>677</v>
+        <v>680</v>
       </c>
       <c r="Q520" t="s">
         <v>675</v>
@@ -22019,28 +21989,28 @@
         <v>26</v>
       </c>
       <c r="D521" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="E521" t="s">
-        <v>538</v>
+        <v>276</v>
       </c>
       <c r="F521" t="s">
         <v>614</v>
       </c>
       <c r="G521" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
       <c r="H521" t="s">
-        <v>669</v>
+        <v>672</v>
       </c>
       <c r="I521" t="s">
         <v>674</v>
       </c>
       <c r="K521">
-        <v>184.015</v>
+        <v>180.4405555555556</v>
       </c>
       <c r="L521">
-        <v>662454</v>
+        <v>649586</v>
       </c>
       <c r="M521" t="s">
         <v>677</v>
@@ -22060,10 +22030,10 @@
         <v>26</v>
       </c>
       <c r="D522" t="s">
-        <v>143</v>
+        <v>112</v>
       </c>
       <c r="E522" t="s">
-        <v>431</v>
+        <v>538</v>
       </c>
       <c r="F522" t="s">
         <v>614</v>
@@ -22075,10 +22045,16 @@
         <v>669</v>
       </c>
       <c r="I522" t="s">
-        <v>675</v>
+        <v>674</v>
+      </c>
+      <c r="K522">
+        <v>184.015</v>
+      </c>
+      <c r="L522">
+        <v>662454</v>
       </c>
       <c r="M522" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="Q522" t="s">
         <v>675</v>
@@ -22095,19 +22071,19 @@
         <v>26</v>
       </c>
       <c r="D523" t="s">
-        <v>27</v>
+        <v>143</v>
       </c>
       <c r="E523" t="s">
-        <v>595</v>
+        <v>431</v>
       </c>
       <c r="F523" t="s">
         <v>614</v>
       </c>
       <c r="G523" t="s">
-        <v>667</v>
+        <v>624</v>
       </c>
       <c r="H523" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="I523" t="s">
         <v>675</v>
@@ -22130,19 +22106,19 @@
         <v>26</v>
       </c>
       <c r="D524" t="s">
-        <v>137</v>
+        <v>27</v>
       </c>
       <c r="E524" t="s">
-        <v>284</v>
+        <v>596</v>
       </c>
       <c r="F524" t="s">
         <v>614</v>
       </c>
       <c r="G524" t="s">
-        <v>617</v>
+        <v>667</v>
       </c>
       <c r="H524" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="I524" t="s">
         <v>675</v>
@@ -22165,31 +22141,25 @@
         <v>26</v>
       </c>
       <c r="D525" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="E525" t="s">
-        <v>434</v>
+        <v>284</v>
       </c>
       <c r="F525" t="s">
         <v>614</v>
       </c>
       <c r="G525" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="H525" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="I525" t="s">
-        <v>674</v>
-      </c>
-      <c r="K525">
-        <v>185.6277777777778</v>
-      </c>
-      <c r="L525">
-        <v>668260</v>
+        <v>675</v>
       </c>
       <c r="M525" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="Q525" t="s">
         <v>675</v>
@@ -22206,31 +22176,31 @@
         <v>26</v>
       </c>
       <c r="D526" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="E526" t="s">
-        <v>596</v>
+        <v>434</v>
       </c>
       <c r="F526" t="s">
         <v>614</v>
       </c>
       <c r="G526" t="s">
-        <v>630</v>
+        <v>621</v>
       </c>
       <c r="H526" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="I526" t="s">
         <v>674</v>
       </c>
       <c r="K526">
-        <v>164.6813888888889</v>
+        <v>185.6277777777778</v>
       </c>
       <c r="L526">
-        <v>592853</v>
+        <v>668260</v>
       </c>
       <c r="M526" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="Q526" t="s">
         <v>675</v>
@@ -22247,7 +22217,7 @@
         <v>26</v>
       </c>
       <c r="D527" t="s">
-        <v>74</v>
+        <v>142</v>
       </c>
       <c r="E527" t="s">
         <v>597</v>
@@ -22256,7 +22226,7 @@
         <v>614</v>
       </c>
       <c r="G527" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="H527" t="s">
         <v>670</v>
@@ -22282,7 +22252,7 @@
         <v>26</v>
       </c>
       <c r="D528" t="s">
-        <v>142</v>
+        <v>110</v>
       </c>
       <c r="E528" t="s">
         <v>598</v>
@@ -22291,16 +22261,22 @@
         <v>614</v>
       </c>
       <c r="G528" t="s">
-        <v>618</v>
+        <v>630</v>
       </c>
       <c r="H528" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="I528" t="s">
-        <v>675</v>
+        <v>674</v>
+      </c>
+      <c r="K528">
+        <v>164.6813888888889</v>
+      </c>
+      <c r="L528">
+        <v>592853</v>
       </c>
       <c r="M528" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="Q528" t="s">
         <v>675</v>
@@ -22317,7 +22293,7 @@
         <v>26</v>
       </c>
       <c r="D529" t="s">
-        <v>58</v>
+        <v>135</v>
       </c>
       <c r="E529" t="s">
         <v>599</v>
@@ -22326,10 +22302,10 @@
         <v>614</v>
       </c>
       <c r="G529" t="s">
-        <v>641</v>
+        <v>668</v>
       </c>
       <c r="H529" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="I529" t="s">
         <v>675</v>
@@ -22352,31 +22328,25 @@
         <v>26</v>
       </c>
       <c r="D530" t="s">
-        <v>118</v>
+        <v>58</v>
       </c>
       <c r="E530" t="s">
-        <v>291</v>
+        <v>600</v>
       </c>
       <c r="F530" t="s">
         <v>614</v>
       </c>
       <c r="G530" t="s">
-        <v>617</v>
+        <v>641</v>
       </c>
       <c r="H530" t="s">
         <v>669</v>
       </c>
       <c r="I530" t="s">
-        <v>674</v>
-      </c>
-      <c r="K530">
-        <v>164.625</v>
-      </c>
-      <c r="L530">
-        <v>592650</v>
+        <v>675</v>
       </c>
       <c r="M530" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="Q530" t="s">
         <v>675</v>
@@ -22393,31 +22363,31 @@
         <v>26</v>
       </c>
       <c r="D531" t="s">
-        <v>38</v>
+        <v>119</v>
       </c>
       <c r="E531" t="s">
-        <v>600</v>
+        <v>291</v>
       </c>
       <c r="F531" t="s">
         <v>614</v>
       </c>
       <c r="G531" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="H531" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="I531" t="s">
         <v>674</v>
       </c>
       <c r="K531">
-        <v>184.5186111111111</v>
+        <v>164.625</v>
       </c>
       <c r="L531">
-        <v>664267</v>
+        <v>592650</v>
       </c>
       <c r="M531" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
       <c r="Q531" t="s">
         <v>675</v>
@@ -22434,13 +22404,13 @@
         <v>26</v>
       </c>
       <c r="D532" t="s">
-        <v>85</v>
+        <v>38</v>
       </c>
       <c r="E532" t="s">
         <v>601</v>
       </c>
       <c r="F532" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="G532" t="s">
         <v>621</v>
@@ -22449,10 +22419,16 @@
         <v>670</v>
       </c>
       <c r="I532" t="s">
-        <v>675</v>
+        <v>674</v>
+      </c>
+      <c r="K532">
+        <v>184.5186111111111</v>
+      </c>
+      <c r="L532">
+        <v>664267</v>
       </c>
       <c r="M532" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="Q532" t="s">
         <v>675</v>
@@ -22469,31 +22445,25 @@
         <v>26</v>
       </c>
       <c r="D533" t="s">
-        <v>153</v>
+        <v>85</v>
       </c>
       <c r="E533" t="s">
         <v>602</v>
       </c>
       <c r="F533" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="G533" t="s">
-        <v>617</v>
+        <v>621</v>
       </c>
       <c r="H533" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="I533" t="s">
-        <v>674</v>
-      </c>
-      <c r="K533">
-        <v>178.3766666666667</v>
-      </c>
-      <c r="L533">
-        <v>642156</v>
+        <v>675</v>
       </c>
       <c r="M533" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="Q533" t="s">
         <v>675</v>
@@ -22510,31 +22480,31 @@
         <v>26</v>
       </c>
       <c r="D534" t="s">
-        <v>72</v>
+        <v>153</v>
       </c>
       <c r="E534" t="s">
-        <v>303</v>
+        <v>603</v>
       </c>
       <c r="F534" t="s">
         <v>614</v>
       </c>
       <c r="G534" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="H534" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="I534" t="s">
         <v>674</v>
       </c>
       <c r="K534">
-        <v>163.5341666666667</v>
+        <v>178.3766666666667</v>
       </c>
       <c r="L534">
-        <v>588723</v>
+        <v>642156</v>
       </c>
       <c r="M534" t="s">
-        <v>679</v>
+        <v>681</v>
       </c>
       <c r="Q534" t="s">
         <v>675</v>
@@ -22551,31 +22521,31 @@
         <v>26</v>
       </c>
       <c r="D535" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="E535" t="s">
-        <v>603</v>
+        <v>303</v>
       </c>
       <c r="F535" t="s">
         <v>614</v>
       </c>
       <c r="G535" t="s">
-        <v>638</v>
+        <v>621</v>
       </c>
       <c r="H535" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="I535" t="s">
         <v>674</v>
       </c>
       <c r="K535">
-        <v>174.7722222222222</v>
+        <v>163.5341666666667</v>
       </c>
       <c r="L535">
-        <v>629180</v>
+        <v>588723</v>
       </c>
       <c r="M535" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="Q535" t="s">
         <v>675</v>
@@ -22592,37 +22562,31 @@
         <v>26</v>
       </c>
       <c r="D536" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="E536" t="s">
-        <v>557</v>
+        <v>604</v>
       </c>
       <c r="F536" t="s">
         <v>614</v>
       </c>
       <c r="G536" t="s">
-        <v>656</v>
+        <v>638</v>
       </c>
       <c r="H536" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="I536" t="s">
         <v>674</v>
       </c>
-      <c r="J536" t="s">
-        <v>676</v>
-      </c>
       <c r="K536">
-        <v>175.7291666666667</v>
+        <v>174.7722222222222</v>
       </c>
       <c r="L536">
-        <v>632625</v>
+        <v>629180</v>
       </c>
       <c r="M536" t="s">
         <v>681</v>
-      </c>
-      <c r="P536" t="s">
-        <v>686</v>
       </c>
       <c r="Q536" t="s">
         <v>675</v>
@@ -22639,31 +22603,37 @@
         <v>26</v>
       </c>
       <c r="D537" t="s">
-        <v>126</v>
+        <v>73</v>
       </c>
       <c r="E537" t="s">
-        <v>314</v>
+        <v>557</v>
       </c>
       <c r="F537" t="s">
         <v>614</v>
       </c>
       <c r="G537" t="s">
-        <v>617</v>
+        <v>656</v>
       </c>
       <c r="H537" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="I537" t="s">
         <v>674</v>
       </c>
+      <c r="J537" t="s">
+        <v>676</v>
+      </c>
       <c r="K537">
-        <v>138.3</v>
+        <v>175.7291666666667</v>
       </c>
       <c r="L537">
-        <v>497880.0000000001</v>
+        <v>632625</v>
       </c>
       <c r="M537" t="s">
-        <v>682</v>
+        <v>681</v>
+      </c>
+      <c r="P537" t="s">
+        <v>686</v>
       </c>
       <c r="Q537" t="s">
         <v>675</v>
@@ -22680,25 +22650,31 @@
         <v>26</v>
       </c>
       <c r="D538" t="s">
-        <v>28</v>
+        <v>127</v>
       </c>
       <c r="E538" t="s">
-        <v>604</v>
+        <v>315</v>
       </c>
       <c r="F538" t="s">
         <v>614</v>
       </c>
       <c r="G538" t="s">
-        <v>634</v>
+        <v>617</v>
       </c>
       <c r="H538" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="I538" t="s">
-        <v>675</v>
+        <v>674</v>
+      </c>
+      <c r="K538">
+        <v>138.3</v>
+      </c>
+      <c r="L538">
+        <v>497880</v>
       </c>
       <c r="M538" t="s">
-        <v>678</v>
+        <v>682</v>
       </c>
       <c r="Q538" t="s">
         <v>675</v>
@@ -22715,7 +22691,7 @@
         <v>26</v>
       </c>
       <c r="D539" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E539" t="s">
         <v>605</v>
@@ -22724,22 +22700,16 @@
         <v>614</v>
       </c>
       <c r="G539" t="s">
-        <v>617</v>
+        <v>634</v>
       </c>
       <c r="H539" t="s">
         <v>670</v>
       </c>
       <c r="I539" t="s">
-        <v>674</v>
-      </c>
-      <c r="K539">
-        <v>174.7808333333333</v>
-      </c>
-      <c r="L539">
-        <v>629211</v>
+        <v>675</v>
       </c>
       <c r="M539" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="Q539" t="s">
         <v>675</v>
@@ -22756,31 +22726,31 @@
         <v>26</v>
       </c>
       <c r="D540" t="s">
-        <v>116</v>
+        <v>36</v>
       </c>
       <c r="E540" t="s">
-        <v>320</v>
+        <v>606</v>
       </c>
       <c r="F540" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="G540" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="H540" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="I540" t="s">
         <v>674</v>
       </c>
       <c r="K540">
-        <v>165.4986111111111</v>
+        <v>174.7808333333333</v>
       </c>
       <c r="L540">
-        <v>595795</v>
+        <v>629211</v>
       </c>
       <c r="M540" t="s">
-        <v>679</v>
+        <v>681</v>
       </c>
       <c r="Q540" t="s">
         <v>675</v>
@@ -22797,31 +22767,31 @@
         <v>26</v>
       </c>
       <c r="D541" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
       <c r="E541" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F541" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="G541" t="s">
-        <v>617</v>
+        <v>621</v>
       </c>
       <c r="H541" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c r="I541" t="s">
         <v>674</v>
       </c>
       <c r="K541">
-        <v>186.8447222222222</v>
+        <v>165.4986111111111</v>
       </c>
       <c r="L541">
-        <v>672641</v>
+        <v>595795</v>
       </c>
       <c r="M541" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
       <c r="Q541" t="s">
         <v>675</v>
@@ -22838,25 +22808,31 @@
         <v>26</v>
       </c>
       <c r="D542" t="s">
-        <v>39</v>
+        <v>94</v>
       </c>
       <c r="E542" t="s">
-        <v>466</v>
+        <v>321</v>
       </c>
       <c r="F542" t="s">
         <v>614</v>
       </c>
       <c r="G542" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="H542" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="I542" t="s">
-        <v>675</v>
+        <v>674</v>
+      </c>
+      <c r="K542">
+        <v>186.8447222222222</v>
+      </c>
+      <c r="L542">
+        <v>672641</v>
       </c>
       <c r="M542" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="Q542" t="s">
         <v>675</v>
@@ -22873,31 +22849,25 @@
         <v>26</v>
       </c>
       <c r="D543" t="s">
-        <v>92</v>
+        <v>39</v>
       </c>
       <c r="E543" t="s">
-        <v>606</v>
+        <v>467</v>
       </c>
       <c r="F543" t="s">
         <v>614</v>
       </c>
       <c r="G543" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="H543" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="I543" t="s">
-        <v>674</v>
-      </c>
-      <c r="K543">
-        <v>185.0066666666667</v>
-      </c>
-      <c r="L543">
-        <v>666024</v>
+        <v>675</v>
       </c>
       <c r="M543" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="Q543" t="s">
         <v>675</v>
@@ -22914,10 +22884,10 @@
         <v>26</v>
       </c>
       <c r="D544" t="s">
-        <v>169</v>
+        <v>92</v>
       </c>
       <c r="E544" t="s">
-        <v>471</v>
+        <v>607</v>
       </c>
       <c r="F544" t="s">
         <v>614</v>
@@ -22929,10 +22899,16 @@
         <v>669</v>
       </c>
       <c r="I544" t="s">
-        <v>675</v>
+        <v>674</v>
+      </c>
+      <c r="K544">
+        <v>185.0066666666667</v>
+      </c>
+      <c r="L544">
+        <v>666024</v>
       </c>
       <c r="M544" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="Q544" t="s">
         <v>675</v>
@@ -22949,19 +22925,19 @@
         <v>26</v>
       </c>
       <c r="D545" t="s">
-        <v>127</v>
+        <v>169</v>
       </c>
       <c r="E545" t="s">
-        <v>329</v>
+        <v>472</v>
       </c>
       <c r="F545" t="s">
         <v>614</v>
       </c>
       <c r="G545" t="s">
-        <v>621</v>
+        <v>625</v>
       </c>
       <c r="H545" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="I545" t="s">
         <v>675</v>
@@ -22984,10 +22960,10 @@
         <v>26</v>
       </c>
       <c r="D546" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="E546" t="s">
-        <v>607</v>
+        <v>329</v>
       </c>
       <c r="F546" t="s">
         <v>614</v>
@@ -23019,10 +22995,10 @@
         <v>26</v>
       </c>
       <c r="D547" t="s">
-        <v>40</v>
+        <v>122</v>
       </c>
       <c r="E547" t="s">
-        <v>338</v>
+        <v>608</v>
       </c>
       <c r="F547" t="s">
         <v>614</v>
@@ -23031,7 +23007,7 @@
         <v>621</v>
       </c>
       <c r="H547" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c r="I547" t="s">
         <v>675</v>
@@ -23054,31 +23030,25 @@
         <v>26</v>
       </c>
       <c r="D548" t="s">
-        <v>91</v>
+        <v>40</v>
       </c>
       <c r="E548" t="s">
-        <v>608</v>
+        <v>338</v>
       </c>
       <c r="F548" t="s">
         <v>614</v>
       </c>
       <c r="G548" t="s">
-        <v>632</v>
+        <v>621</v>
       </c>
       <c r="H548" t="s">
         <v>669</v>
       </c>
       <c r="I548" t="s">
-        <v>674</v>
-      </c>
-      <c r="K548">
-        <v>169.0716666666667</v>
-      </c>
-      <c r="L548">
-        <v>608658</v>
+        <v>675</v>
       </c>
       <c r="M548" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="Q548" t="s">
         <v>675</v>
@@ -23095,16 +23065,16 @@
         <v>26</v>
       </c>
       <c r="D549" t="s">
-        <v>161</v>
+        <v>91</v>
       </c>
       <c r="E549" t="s">
-        <v>342</v>
+        <v>609</v>
       </c>
       <c r="F549" t="s">
         <v>614</v>
       </c>
       <c r="G549" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="H549" t="s">
         <v>669</v>
@@ -23113,13 +23083,13 @@
         <v>674</v>
       </c>
       <c r="K549">
-        <v>183.7677777777778</v>
+        <v>169.0716666666667</v>
       </c>
       <c r="L549">
-        <v>661564</v>
+        <v>608658</v>
       </c>
       <c r="M549" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
       <c r="Q549" t="s">
         <v>675</v>
@@ -23136,28 +23106,28 @@
         <v>26</v>
       </c>
       <c r="D550" t="s">
-        <v>131</v>
+        <v>161</v>
       </c>
       <c r="E550" t="s">
-        <v>609</v>
+        <v>342</v>
       </c>
       <c r="F550" t="s">
         <v>614</v>
       </c>
       <c r="G550" t="s">
-        <v>641</v>
+        <v>636</v>
       </c>
       <c r="H550" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="I550" t="s">
         <v>674</v>
       </c>
       <c r="K550">
-        <v>183.0261111111111</v>
+        <v>183.7677777777778</v>
       </c>
       <c r="L550">
-        <v>658894</v>
+        <v>661564</v>
       </c>
       <c r="M550" t="s">
         <v>677</v>
@@ -23177,7 +23147,7 @@
         <v>26</v>
       </c>
       <c r="D551" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="E551" t="s">
         <v>610</v>
@@ -23186,19 +23156,19 @@
         <v>614</v>
       </c>
       <c r="G551" t="s">
-        <v>617</v>
+        <v>641</v>
       </c>
       <c r="H551" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="I551" t="s">
         <v>674</v>
       </c>
       <c r="K551">
-        <v>183.0975</v>
+        <v>183.0261111111111</v>
       </c>
       <c r="L551">
-        <v>659151</v>
+        <v>658894</v>
       </c>
       <c r="M551" t="s">
         <v>677</v>
@@ -23218,7 +23188,7 @@
         <v>26</v>
       </c>
       <c r="D552" t="s">
-        <v>155</v>
+        <v>129</v>
       </c>
       <c r="E552" t="s">
         <v>611</v>
@@ -23227,22 +23197,25 @@
         <v>614</v>
       </c>
       <c r="G552" t="s">
-        <v>632</v>
+        <v>617</v>
       </c>
       <c r="H552" t="s">
         <v>669</v>
       </c>
       <c r="I552" t="s">
-        <v>675</v>
+        <v>674</v>
+      </c>
+      <c r="K552">
+        <v>183.0975</v>
+      </c>
+      <c r="L552">
+        <v>659151</v>
       </c>
       <c r="M552" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="Q552" t="s">
-        <v>674</v>
-      </c>
-      <c r="R552">
-        <v>23858</v>
+        <v>675</v>
       </c>
     </row>
     <row r="553" spans="1:18">
@@ -23256,34 +23229,31 @@
         <v>26</v>
       </c>
       <c r="D553" t="s">
-        <v>32</v>
+        <v>155</v>
       </c>
       <c r="E553" t="s">
-        <v>576</v>
+        <v>612</v>
       </c>
       <c r="F553" t="s">
         <v>614</v>
       </c>
       <c r="G553" t="s">
-        <v>618</v>
+        <v>632</v>
       </c>
       <c r="H553" t="s">
         <v>669</v>
       </c>
       <c r="I553" t="s">
-        <v>674</v>
-      </c>
-      <c r="K553">
-        <v>183.0180555555555</v>
-      </c>
-      <c r="L553">
-        <v>658865</v>
+        <v>675</v>
       </c>
       <c r="M553" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="Q553" t="s">
-        <v>675</v>
+        <v>674</v>
+      </c>
+      <c r="R553">
+        <v>23858</v>
       </c>
     </row>
     <row r="554" spans="1:18">
@@ -23297,16 +23267,16 @@
         <v>26</v>
       </c>
       <c r="D554" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="E554" t="s">
-        <v>350</v>
+        <v>576</v>
       </c>
       <c r="F554" t="s">
         <v>614</v>
       </c>
       <c r="G554" t="s">
-        <v>625</v>
+        <v>618</v>
       </c>
       <c r="H554" t="s">
         <v>669</v>
@@ -23315,10 +23285,10 @@
         <v>674</v>
       </c>
       <c r="K554">
-        <v>185.0066666666667</v>
+        <v>183.0180555555555</v>
       </c>
       <c r="L554">
-        <v>666024</v>
+        <v>658865</v>
       </c>
       <c r="M554" t="s">
         <v>677</v>
@@ -23338,16 +23308,16 @@
         <v>26</v>
       </c>
       <c r="D555" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E555" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F555" t="s">
         <v>614</v>
       </c>
       <c r="G555" t="s">
-        <v>617</v>
+        <v>625</v>
       </c>
       <c r="H555" t="s">
         <v>669</v>
@@ -23356,10 +23326,10 @@
         <v>674</v>
       </c>
       <c r="K555">
-        <v>184.4086111111111</v>
+        <v>185.0066666666667</v>
       </c>
       <c r="L555">
-        <v>663871</v>
+        <v>666024</v>
       </c>
       <c r="M555" t="s">
         <v>677</v>
@@ -23379,25 +23349,31 @@
         <v>26</v>
       </c>
       <c r="D556" t="s">
-        <v>135</v>
+        <v>50</v>
       </c>
       <c r="E556" t="s">
-        <v>612</v>
+        <v>351</v>
       </c>
       <c r="F556" t="s">
         <v>614</v>
       </c>
       <c r="G556" t="s">
-        <v>668</v>
+        <v>617</v>
       </c>
       <c r="H556" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="I556" t="s">
-        <v>675</v>
+        <v>674</v>
+      </c>
+      <c r="K556">
+        <v>184.4086111111111</v>
+      </c>
+      <c r="L556">
+        <v>663871</v>
       </c>
       <c r="M556" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="Q556" t="s">
         <v>675</v>

</xml_diff>